<commit_message>
Adding read_input_file() to core.py and created file reader.py
</commit_message>
<xml_diff>
--- a/Input Template.xlsx
+++ b/Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Synchro Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A07D57D-D12B-4F54-B6DE-32DC20FC7BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8555FE36-610C-4B4C-A256-6F36D7D0C7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="-1935" windowWidth="14400" windowHeight="15600" xr2:uid="{B935739B-1E8B-4825-9ECD-1B8D98B964E5}"/>
   </bookViews>
@@ -203,10 +203,10 @@
     <t>Step 3C</t>
   </si>
   <si>
-    <t>REPEAT</t>
-  </si>
-  <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>*REPEAT*</t>
   </si>
 </sst>
 </file>
@@ -924,9 +924,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -938,6 +935,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -1188,14 +1188,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC750F6C-98FF-418C-9ABC-56FF6AE1D7AD}">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="70" customWidth="1"/>
-    <col min="2" max="2" width="20" style="70" customWidth="1"/>
+    <col min="2" max="2" width="9" style="70" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="70" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="70" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="70" customWidth="1"/>
@@ -1215,7 +1215,7 @@
     <col min="19" max="19" width="13.21875" style="70" customWidth="1"/>
     <col min="22" max="22" width="11.5546875" style="70" customWidth="1"/>
     <col min="23" max="25" width="8.88671875" style="70"/>
-    <col min="26" max="26" width="25.109375" style="70" customWidth="1"/>
+    <col min="26" max="26" width="10.21875" style="70" customWidth="1"/>
     <col min="28" max="16384" width="8.88671875" style="70"/>
   </cols>
   <sheetData>
@@ -1385,7 +1385,7 @@
       <c r="AC3" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" s="83" t="s">
+      <c r="AD3" s="82" t="s">
         <v>50</v>
       </c>
       <c r="AE3" t="s">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="Z4" s="70"/>
       <c r="AC4" s="70"/>
-      <c r="AD4" s="84" t="s">
+      <c r="AD4" s="83" t="s">
         <v>50</v>
       </c>
       <c r="AE4" t="s">
@@ -1487,7 +1487,7 @@
       <c r="Z5" s="70"/>
       <c r="AB5" s="70"/>
       <c r="AC5" s="70"/>
-      <c r="AD5" s="85" t="s">
+      <c r="AD5" s="84" t="s">
         <v>50</v>
       </c>
       <c r="AE5" t="s">
@@ -1539,8 +1539,8 @@
       <c r="X6" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="Z6" s="82" t="s">
-        <v>56</v>
+      <c r="Z6" s="86" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:31" customFormat="1" x14ac:dyDescent="0.3">
@@ -2394,8 +2394,8 @@
       <c r="O26" s="66"/>
       <c r="P26" s="67"/>
       <c r="Q26" s="68"/>
-      <c r="S26" s="86" t="s">
-        <v>57</v>
+      <c r="S26" s="85" t="s">
+        <v>56</v>
       </c>
       <c r="U26" s="74" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Updated README.md and added requirements.txt
</commit_message>
<xml_diff>
--- a/Input Template.xlsx
+++ b/Input Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Synchro Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8076E5E5-6B3C-49DC-9D98-74B2F5E57717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A050B8-8CE9-4ED7-8F1B-72BAA2443105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="-1935" windowWidth="14400" windowHeight="15600" xr2:uid="{B935739B-1E8B-4825-9ECD-1B8D98B964E5}"/>
+    <workbookView minimized="1" xWindow="37410" yWindow="-930" windowWidth="13515" windowHeight="10545" xr2:uid="{B935739B-1E8B-4825-9ECD-1B8D98B964E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -1190,7 +1190,7 @@
   <dimension ref="A1:AE46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>

</xml_diff>